<commit_message>
Change png map with bits and bytes
</commit_message>
<xml_diff>
--- a/Backlogs/backlog_s3.xlsx
+++ b/Backlogs/backlog_s3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-4540" yWindow="-21160" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="3700" yWindow="1180" windowWidth="38400" windowHeight="21160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlogs" sheetId="2" r:id="rId1"/>
@@ -450,7 +450,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="144">
+  <cellStyleXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -557,6 +557,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -652,7 +674,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="144">
+  <cellStyles count="166">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -724,6 +746,17 @@
     <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -795,6 +828,17 @@
     <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="105"/>
   </cellStyles>
@@ -990,16 +1034,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7.105427357601E-15</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.105427357601E-15</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.105427357601E-15</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.105427357601E-15</c:v>
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1076,16 +1123,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>90.00000000000001</c:v>
+                  <c:v>84.43333333333329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68.95000000000001</c:v>
+                  <c:v>65.83333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47.90000000000001</c:v>
+                  <c:v>47.23333333333332</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.85000000000001</c:v>
+                  <c:v>28.63333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.03333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1168,11 +1218,11 @@
         </c:upDownBars>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127154968"/>
-        <c:axId val="2127158248"/>
+        <c:axId val="2139675672"/>
+        <c:axId val="2139678920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127154968"/>
+        <c:axId val="2139675672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1207,7 +1257,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127158248"/>
+        <c:crossAx val="2139678920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1217,7 +1267,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127158248"/>
+        <c:axId val="2139678920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,7 +1312,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127154968"/>
+        <c:crossAx val="2139675672"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1421,6 +1471,9 @@
                 <c:pt idx="2">
                   <c:v>22.0</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1458,6 +1511,9 @@
                 <c:pt idx="2">
                   <c:v>21.5</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.7</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1471,8 +1527,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="2126134616"/>
-        <c:axId val="2126138248"/>
+        <c:axId val="2131578728"/>
+        <c:axId val="2131582296"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1501,16 +1557,16 @@
                 <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>20.43333333333333</c:v>
+                  <c:v>17.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.43333333333333</c:v>
+                  <c:v>17.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.43333333333333</c:v>
+                  <c:v>17.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.43333333333333</c:v>
+                  <c:v>17.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1541,16 +1597,16 @@
                 <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>20.43333333333333</c:v>
+                  <c:v>17.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.43333333333333</c:v>
+                  <c:v>17.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.43333333333333</c:v>
+                  <c:v>17.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.43333333333333</c:v>
+                  <c:v>17.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1581,16 +1637,16 @@
                 <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>20.43333333333333</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.43333333333333</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.43333333333333</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.43333333333333</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1607,11 +1663,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2126134616"/>
-        <c:axId val="2126138248"/>
+        <c:axId val="2131578728"/>
+        <c:axId val="2131582296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2126134616"/>
+        <c:axId val="2131578728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1646,7 +1702,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126138248"/>
+        <c:crossAx val="2131582296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1656,7 +1712,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126138248"/>
+        <c:axId val="2131582296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,7 +1757,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126134616"/>
+        <c:crossAx val="2131578728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2221,7 +2277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -2820,8 +2876,8 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2829,13 +2885,13 @@
     <col min="1" max="1" width="11.83203125" style="5" customWidth="1"/>
     <col min="2" max="4" width="8.83203125" style="5"/>
     <col min="5" max="5" width="14.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="5" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="5.5" style="5" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" style="5" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="4.33203125" style="5" hidden="1" customWidth="1"/>
-    <col min="11" max="13" width="6.83203125" style="5" hidden="1" customWidth="1"/>
-    <col min="14" max="16" width="9.1640625" style="5" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5" style="5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="5" customWidth="1"/>
+    <col min="7" max="8" width="5.5" style="5" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="4.33203125" style="5" customWidth="1"/>
+    <col min="11" max="13" width="6.83203125" style="5" customWidth="1"/>
+    <col min="14" max="16" width="9.1640625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="5" customWidth="1"/>
     <col min="18" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
@@ -2855,8 +2911,7 @@
         <v>33</v>
       </c>
       <c r="G3" s="6">
-        <f>IF(COUNT(B28:B31)=0,1,COUNT(B28:B31))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -2874,7 +2929,7 @@
       </c>
       <c r="G4" s="6">
         <f>IF(COUNT(D28:D31)=0,1,COUNT(D28:D31)+1)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -2883,7 +2938,7 @@
       </c>
       <c r="G5" s="6">
         <f>IF(G4&gt;D4,G4-D4,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z5" s="7"/>
     </row>
@@ -2905,7 +2960,7 @@
         <v>40</v>
       </c>
       <c r="D7" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="Z7" s="7"/>
     </row>
@@ -2917,7 +2972,7 @@
       <c r="B8" s="23"/>
       <c r="D8" s="9">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,TrendOffset,0,SprintsInTrend,1)))</f>
-        <v>20.433333333333334</v>
+        <v>19.266666666666666</v>
       </c>
       <c r="Z8" s="7"/>
     </row>
@@ -2927,14 +2982,14 @@
       </c>
       <c r="D9" s="9">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,1,0,SprintCount,1)))</f>
-        <v>20.433333333333334</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>42</v>
       </c>
       <c r="G9" s="6">
         <f ca="1">IF(M28="",1,COUNT(M28:M110))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Z9" s="7"/>
     </row>
@@ -2943,8 +2998,8 @@
         <v>43</v>
       </c>
       <c r="D10" s="9">
-        <f ca="1">IF(D28="","",AVERAGE(LastEight))</f>
-        <v>20.433333333333334</v>
+        <f>IF(D28="","",AVERAGE(D28:D32))</f>
+        <v>17.600000000000001</v>
       </c>
       <c r="Z10" s="7"/>
     </row>
@@ -2953,8 +3008,8 @@
         <v>44</v>
       </c>
       <c r="D11" s="9">
-        <f ca="1">IF(D28="","",IF(TrendSprintCount&lt;4,D10,AVERAGE(SMALL(LastEight,1),SMALL(LastEight,2),SMALL(LastEight,3))))</f>
-        <v>20.433333333333334</v>
+        <f>IF(D28="","",IF(TrendSprintCount&lt;4,D10,AVERAGE(SMALL(D28:D32,1),SMALL(D28:D32,2),SMALL(D28:D32,3))))</f>
+        <v>15.299999999999999</v>
       </c>
       <c r="Z11" s="7"/>
     </row>
@@ -2964,7 +3019,7 @@
       </c>
       <c r="D12" s="9">
         <f ca="1">IF(M29="","",M28-M29)</f>
-        <v>21.049999999999997</v>
+        <v>18.59999999999998</v>
       </c>
       <c r="Z12" s="7"/>
     </row>
@@ -2985,7 +3040,7 @@
       </c>
       <c r="D15" s="11">
         <f>IF(D7="",0,ROUNDUP(D3/D7*0.6,0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -2994,7 +3049,7 @@
       </c>
       <c r="D16" s="11">
         <f>IF(D7="",0,ROUNDUP(D3/D7,0))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -3003,14 +3058,14 @@
       </c>
       <c r="D17" s="11">
         <f>IF(D7="",0,ROUNDUP(D3/D7*1.6,0))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>51</v>
       </c>
       <c r="G17" s="5">
         <f>IF(OR(D28="",D29=""),1,STDEV(D28:D31))</f>
-        <v>1.1590225767142479</v>
+        <v>2.5488559525141214</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -3030,14 +3085,14 @@
       </c>
       <c r="D19" s="11">
         <f ca="1">IF(D9="","",IF(LastRealized="",ROUNDUP(LastPlanned/D9+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D9,0)+SprintCount))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>53</v>
       </c>
       <c r="G19" s="5">
         <f ca="1">LastPlanned</f>
-        <v>26.699999999999996</v>
+        <v>10.999999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -3046,14 +3101,14 @@
       </c>
       <c r="D20" s="11">
         <f ca="1">IF(D10="","",IF(LastRealized="",ROUNDUP(LastPlanned/D10+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D10,0)+SprintCount))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>54</v>
       </c>
       <c r="G20" s="5">
         <f ca="1">LastRealized</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -3062,7 +3117,7 @@
       </c>
       <c r="D21" s="11">
         <f ca="1">IF(D11="","",IF(LastRealized="",ROUNDUP(LastPlanned/D11+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D11,0)+SprintCount))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -3181,11 +3236,11 @@
         <v>88</v>
       </c>
       <c r="G28" s="6">
-        <f t="shared" ref="G28:G31" si="0">F28</f>
+        <f t="shared" ref="G28:G32" si="0">F28</f>
         <v>88</v>
       </c>
       <c r="H28" s="6">
-        <f t="shared" ref="H28:H31" si="1">I28</f>
+        <f t="shared" ref="H28:H32" si="1">I28</f>
         <v>0</v>
       </c>
       <c r="I28" s="6">
@@ -3196,28 +3251,28 @@
         <v>88</v>
       </c>
       <c r="L28" s="6">
-        <f t="shared" ref="L28:L31" ca="1" si="3">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),A28)&lt;N28,N28,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),A28))</f>
-        <v>90.000000000000014</v>
+        <f t="shared" ref="L28:L32" ca="1" si="3">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),A28)&lt;N28,N28,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),A28))</f>
+        <v>84.433333333333294</v>
       </c>
       <c r="M28" s="6">
         <f ca="1">L28</f>
-        <v>90.000000000000014</v>
+        <v>84.433333333333294</v>
       </c>
       <c r="N28" s="6">
         <f t="shared" ref="I28:N51" ca="1" si="4">OFFSET($I$27,TrendSprintCount,0,1,1)</f>
-        <v>7.1054273576010019E-15</v>
+        <v>0</v>
       </c>
       <c r="O28" s="21">
         <f t="shared" ref="O28:O31" ca="1" si="5">D$9</f>
-        <v>20.433333333333334</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="P28" s="21">
-        <f t="shared" ref="P28:P31" ca="1" si="6">D$10</f>
-        <v>20.433333333333334</v>
+        <f t="shared" ref="P28:P31" si="6">D$10</f>
+        <v>17.600000000000001</v>
       </c>
       <c r="Q28" s="21">
-        <f t="shared" ref="Q28:Q31" ca="1" si="7">D$11</f>
-        <v>20.433333333333334</v>
+        <f t="shared" ref="Q28:Q31" si="7">D$11</f>
+        <v>15.299999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -3239,7 +3294,7 @@
         <v>88</v>
       </c>
       <c r="F29" s="6">
-        <f t="shared" ref="F29:F31" si="8">IF(B29="",IF(B28="","",IF(D28="","",I28)),IF(AND(D28="",C28=""),"",IF(AND(D28="",C28&lt;&gt;""),IF(I28&gt;F28,F28,I28),F28-D28)))</f>
+        <f t="shared" ref="F29:G32" si="8">IF(B29="",IF(B28="","",IF(D28="","",I28)),IF(AND(D28="",C28=""),"",IF(AND(D28="",C28&lt;&gt;""),IF(I28&gt;F28,F28,I28),F28-D28)))</f>
         <v>68.8</v>
       </c>
       <c r="G29" s="6">
@@ -3260,27 +3315,27 @@
       </c>
       <c r="L29" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>68.950000000000017</v>
+        <v>65.833333333333314</v>
       </c>
       <c r="M29" s="6">
         <f ca="1">IF(L29=L28,"",L29)</f>
-        <v>68.950000000000017</v>
+        <v>65.833333333333314</v>
       </c>
       <c r="N29" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
+        <v>0</v>
       </c>
       <c r="O29" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>20.433333333333334</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="P29" s="21">
-        <f t="shared" ca="1" si="6"/>
-        <v>20.433333333333334</v>
+        <f t="shared" si="6"/>
+        <v>17.600000000000001</v>
       </c>
       <c r="Q29" s="21">
-        <f t="shared" ca="1" si="7"/>
-        <v>20.433333333333334</v>
+        <f t="shared" si="7"/>
+        <v>15.299999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -3323,27 +3378,27 @@
       </c>
       <c r="L30" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>47.900000000000006</v>
+        <v>47.23333333333332</v>
       </c>
       <c r="M30" s="6">
         <f t="shared" ref="H30:M51" ca="1" si="9">IF(L30=L29,"",L30)</f>
-        <v>47.900000000000006</v>
+        <v>47.23333333333332</v>
       </c>
       <c r="N30" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
+        <v>0</v>
       </c>
       <c r="O30" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>20.433333333333334</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="P30" s="21">
-        <f t="shared" ca="1" si="6"/>
-        <v>20.433333333333334</v>
+        <f t="shared" si="6"/>
+        <v>17.600000000000001</v>
       </c>
       <c r="Q30" s="21">
-        <f t="shared" ca="1" si="7"/>
-        <v>20.433333333333334</v>
+        <f t="shared" si="7"/>
+        <v>15.299999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -3354,8 +3409,12 @@
         <f>B30-D30</f>
         <v>26.699999999999996</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
+      <c r="C31" s="20">
+        <v>18</v>
+      </c>
+      <c r="D31" s="20">
+        <v>15.7</v>
+      </c>
       <c r="E31" s="19">
         <f>IF(B31="","",IF(D30="",E30,B31+SUM(D$28:D30)))</f>
         <v>88</v>
@@ -3382,628 +3441,246 @@
       </c>
       <c r="L31" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>26.850000000000009</v>
+        <v>28.633333333333326</v>
       </c>
       <c r="M31" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>26.850000000000009</v>
+        <v>28.633333333333326</v>
       </c>
       <c r="N31" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
+        <v>0</v>
       </c>
       <c r="O31" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>20.433333333333334</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="P31" s="21">
-        <f t="shared" ca="1" si="6"/>
-        <v>20.433333333333334</v>
+        <f t="shared" si="6"/>
+        <v>17.600000000000001</v>
       </c>
       <c r="Q31" s="21">
-        <f t="shared" ca="1" si="7"/>
-        <v>20.433333333333334</v>
+        <f t="shared" si="7"/>
+        <v>15.299999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:17">
-      <c r="F32" s="5">
-        <f t="shared" si="2"/>
+      <c r="A32" s="19">
+        <v>5</v>
+      </c>
+      <c r="B32" s="20">
+        <f>B31-D31</f>
+        <v>10.999999999999996</v>
+      </c>
+      <c r="C32" s="20">
+        <v>11</v>
+      </c>
+      <c r="D32" s="20">
+        <v>11</v>
+      </c>
+      <c r="E32" s="19">
+        <f>IF(B32="","",IF(D31="",E31,B32+SUM(D$28:D31)))</f>
+        <v>88</v>
+      </c>
+      <c r="F32" s="6">
+        <f t="shared" ref="F32" si="10">IF(B32="",IF(B31="","",IF(D31="","",I31)),IF(AND(D31="",C31=""),"",IF(AND(D31="",C31&lt;&gt;""),IF(I31&gt;F31,F31,I31),F31-D31)))</f>
+        <v>10.999999999999996</v>
+      </c>
+      <c r="G32" s="6">
+        <f t="shared" ref="G32" si="11">F32</f>
+        <v>10.999999999999996</v>
+      </c>
+      <c r="H32" s="6">
+        <f t="shared" ref="H32" si="12">I32</f>
         <v>0</v>
       </c>
-      <c r="G32" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I32,I32,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H32" s="6" t="e">
-        <f ca="1">IF(G32=L31,"",G32)</f>
-        <v>#REF!</v>
-      </c>
       <c r="I32" s="6">
+        <f>IF(B32="",IF(B31="","",IF(D31="","",F31-D31)),IF(AND(C31="",D31=""),"",IF(AND(D31="",C31&lt;&gt;""),IF(I31&gt;F31,I31-C31,F31-C31),B$28-B32-SUM(D$28:D31))))</f>
+        <v>0</v>
+      </c>
+      <c r="K32" s="5">
+        <f t="shared" ref="K32" si="13">IF(F32&lt;I32,I32,F32)</f>
+        <v>10.999999999999996</v>
+      </c>
+      <c r="L32" s="6">
+        <f t="shared" ref="L32" ca="1" si="14">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),A32)&lt;N32,N32,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),A32))</f>
+        <v>10.033333333333331</v>
+      </c>
+      <c r="M32" s="6">
+        <f t="shared" ref="M32" ca="1" si="15">IF(L32=L31,"",L32)</f>
+        <v>10.033333333333331</v>
+      </c>
+      <c r="N32" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J32" s="21">
-        <f t="shared" ref="J32:J51" ca="1" si="10">D$9</f>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K32" s="21">
-        <f t="shared" ref="K32:K51" ca="1" si="11">D$10</f>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L32" s="21">
-        <f t="shared" ref="L32:L51" ca="1" si="12">D$11</f>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="33" spans="6:12">
-      <c r="F33" s="5">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G33" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I33,I33,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H33" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I33" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J33" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K33" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L33" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="34" spans="6:12">
-      <c r="F34" s="5">
-        <f t="shared" si="2"/>
+      <c r="O32" s="21">
+        <f t="shared" ref="O32" ca="1" si="16">D$9</f>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="P32" s="21">
+        <f t="shared" ref="P32" si="17">D$10</f>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="Q32" s="21">
+        <f t="shared" ref="Q32" si="18">D$11</f>
+        <v>15.299999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12">
+      <c r="B33" s="5">
         <v>0</v>
       </c>
-      <c r="G34" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I34,I34,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H34" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I34" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J34" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K34" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L34" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="35" spans="6:12">
-      <c r="F35" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G35" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I35,I35,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H35" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I35" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J35" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K35" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L35" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="36" spans="6:12">
-      <c r="F36" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G36" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I36,I36,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H36" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I36" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J36" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K36" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L36" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="37" spans="6:12">
-      <c r="F37" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G37" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I37,I37,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H37" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I37" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J37" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K37" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L37" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="38" spans="6:12">
-      <c r="F38" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G38" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I38,I38,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H38" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I38" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J38" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K38" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L38" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="39" spans="6:12">
-      <c r="F39" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G39" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I39,I39,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H39" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I39" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J39" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K39" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L39" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="40" spans="6:12">
-      <c r="F40" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G40" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I40,I40,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H40" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I40" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J40" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K40" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L40" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="41" spans="6:12">
-      <c r="F41" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G41" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I41,I41,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H41" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I41" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J41" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K41" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L41" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="42" spans="6:12">
-      <c r="F42" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G42" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I42,I42,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H42" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I42" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J42" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K42" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L42" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="43" spans="6:12">
-      <c r="F43" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G43" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I43,I43,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H43" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I43" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J43" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K43" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L43" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="44" spans="6:12">
-      <c r="F44" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G44" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I44,I44,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H44" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I44" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J44" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K44" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L44" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="45" spans="6:12">
-      <c r="F45" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G45" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I45,I45,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H45" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I45" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J45" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K45" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L45" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="46" spans="6:12">
-      <c r="F46" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G46" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I46,I46,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H46" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I46" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J46" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K46" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L46" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="47" spans="6:12">
-      <c r="F47" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G47" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I47,I47,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H47" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I47" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J47" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K47" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L47" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="48" spans="6:12">
-      <c r="F48" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G48" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I48,I48,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H48" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I48" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J48" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K48" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L48" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="49" spans="6:12">
-      <c r="F49" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G49" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I49,I49,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H49" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I49" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J49" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K49" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L49" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="50" spans="6:12">
-      <c r="F50" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G50" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I50,I50,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H50" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I50" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J50" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K50" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L50" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
-    </row>
-    <row r="51" spans="6:12">
-      <c r="F51" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G51" s="6" t="e">
-        <f ca="1">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!)&lt;I51,I51,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H51" s="6" t="e">
-        <f t="shared" ca="1" si="9"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I51" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-      <c r="J51" s="21">
-        <f t="shared" ca="1" si="10"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="K51" s="21">
-        <f t="shared" ca="1" si="11"/>
-        <v>20.433333333333334</v>
-      </c>
-      <c r="L51" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>20.433333333333334</v>
-      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+    </row>
+    <row r="34" spans="2:12">
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+    </row>
+    <row r="35" spans="2:12">
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+    </row>
+    <row r="36" spans="2:12">
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+    </row>
+    <row r="37" spans="2:12">
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+    </row>
+    <row r="38" spans="2:12">
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+    </row>
+    <row r="39" spans="2:12">
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+    </row>
+    <row r="40" spans="2:12">
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+    </row>
+    <row r="41" spans="2:12">
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+    </row>
+    <row r="42" spans="2:12">
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+    </row>
+    <row r="43" spans="2:12">
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+    </row>
+    <row r="44" spans="2:12">
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+    </row>
+    <row r="45" spans="2:12">
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+    </row>
+    <row r="46" spans="2:12">
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+    </row>
+    <row r="47" spans="2:12">
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+    </row>
+    <row r="48" spans="2:12">
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
+    </row>
+    <row r="49" spans="7:12">
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
+    </row>
+    <row r="50" spans="7:12">
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+    </row>
+    <row r="51" spans="7:12">
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>